<commit_message>
avanzando en el datagrama
</commit_message>
<xml_diff>
--- a/p2/database/dades.xlsx
+++ b/p2/database/dades.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Rajah</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Foot_wear</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -202,9 +205,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +490,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,136 +502,180 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f ca="1">RANDBETWEEN(18,60)</f>
-        <v>60</v>
+      <c r="F1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D9" ca="1" si="0">RANDBETWEEN(18,60)</f>
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
       </c>
       <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+      <c r="F4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+      <c r="F5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>15</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>17</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ca="1" si="0"/>
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -643,109 +689,165 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
+      <c r="B1">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>26</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +860,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,11 +874,11 @@
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1">
         <v>2013</v>
@@ -789,11 +891,11 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" ca="1" si="0">RANDBETWEEN(1,30)</f>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C9" ca="1" si="1">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>2013</v>
@@ -806,11 +908,11 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>2013</v>
@@ -823,11 +925,11 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>2013</v>
@@ -840,11 +942,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>2013</v>
@@ -857,11 +959,11 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -874,11 +976,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>2013</v>
@@ -891,11 +993,11 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>2013</v>
@@ -908,11 +1010,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>2013</v>
@@ -925,122 +1027,177 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
+      <c r="B1">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(A1,1)</f>
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">SUM(A2,1)</f>
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1051,94 +1208,121 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">A2+1</f>
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1149,18 +1333,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1168,19 +1352,20 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <f ca="1">RANDBETWEEN(10,20)</f>
+        <v>11</v>
       </c>
       <c r="D1">
-        <f ca="1">RANDBETWEEN(10,20)</f>
-        <v>16</v>
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>2</v>
       </c>
       <c r="E1">
-        <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>8</v>
       </c>
       <c r="F1">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <f ca="1">RANDBETWEEN(1,9)</f>
+        <v>2</v>
       </c>
       <c r="G1">
         <f ca="1">RANDBETWEEN(1,9)</f>
@@ -1188,547 +1373,500 @@
       </c>
       <c r="H1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J1">
         <f ca="1">RANDBETWEEN(1,9)</f>
         <v>7</v>
       </c>
-      <c r="K1">
-        <f ca="1">RANDBETWEEN(1,9)</f>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(10,20)</f>
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D13" ca="1" si="1">RANDBETWEEN(1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E13" ca="1" si="2">RANDBETWEEN(1,10)</f>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:J13" ca="1" si="3">RANDBETWEEN(1,9)</f>
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>A1+1</f>
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="H2">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D13" ca="1" si="0">RANDBETWEEN(10,20)</f>
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E13" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F13" ca="1" si="2">RANDBETWEEN(1,10)</f>
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:K13" ca="1" si="3">RANDBETWEEN(1,9)</f>
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="J2">
+      <c r="D3">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I4">
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="K2">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A13" si="4">A2+1</f>
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
+      <c r="J4">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
-      <c r="G3">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="F6">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G8">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="I4">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
+      <c r="H8">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="C9">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
-      <c r="E5">
+      <c r="D9">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="J9">
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="J5">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F12">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="J6">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="B7">
+      <c r="G12">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="J12">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="K7">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="C13">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="E13">
         <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="J9">
+      <c r="F13">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H13">
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="I13">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="J11">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="K11">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="K13">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All runs well, except slicer of the year
</commit_message>
<xml_diff>
--- a/p2/database/dades.xlsx
+++ b/p2/database/dades.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maikell\Documents\GitHub\ADB\p2\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16608" windowHeight="9432" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="1" r:id="rId1"/>
@@ -19,9 +14,9 @@
     <sheet name="tienda" sheetId="5" r:id="rId5"/>
     <sheet name="ventas" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Rajah</t>
   </si>
@@ -167,16 +162,13 @@
   </si>
   <si>
     <t>Foot_wear</t>
-  </si>
-  <si>
-    <t>z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -267,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,26 +471,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>1</v>
       </c>
@@ -518,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2</v>
       </c>
@@ -538,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>3</v>
       </c>
@@ -558,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>4</v>
       </c>
@@ -578,7 +570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>5</v>
       </c>
@@ -598,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>6</v>
       </c>
@@ -618,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>7</v>
       </c>
@@ -638,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>8</v>
       </c>
@@ -658,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>9</v>
       </c>
@@ -685,19 +677,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>1</v>
       </c>
@@ -714,7 +706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>2</v>
       </c>
@@ -731,7 +723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>3</v>
       </c>
@@ -748,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>4</v>
       </c>
@@ -765,7 +757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>5</v>
       </c>
@@ -782,7 +774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>6</v>
       </c>
@@ -799,7 +791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>7</v>
       </c>
@@ -816,7 +808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>8</v>
       </c>
@@ -833,7 +825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>9</v>
       </c>
@@ -856,165 +848,165 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D1">
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <f>SUM(A1,1)</f>
         <v>2</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" ca="1" si="0">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C9" ca="1" si="1">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <f t="shared" ref="A3:A8" si="2">SUM(A2,1)</f>
         <v>3</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>2013</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2013</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>2013</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <f>SUM(A8,1)</f>
         <v>9</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>2013</v>
@@ -1026,21 +1018,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1057,7 +1049,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <f>SUM(A1,1)</f>
         <v>2</v>
@@ -1075,7 +1067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">SUM(A2,1)</f>
         <v>3</v>
@@ -1093,7 +1085,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1111,7 +1103,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1129,7 +1121,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1147,7 +1139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1165,7 +1157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1183,7 +1175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1207,19 +1199,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1230,7 +1222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -1242,7 +1234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">A2+1</f>
         <v>3</v>
@@ -1254,7 +1246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1266,7 +1258,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1278,7 +1270,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1290,7 +1282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1302,7 +1294,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1314,7 +1306,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1332,19 +1324,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1353,38 +1345,38 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(10,20)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J1">
         <f ca="1">RANDBETWEEN(1,9)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1393,7 +1385,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(10,20)</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D13" ca="1" si="1">RANDBETWEEN(1,4)</f>
@@ -1401,30 +1393,30 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E13" ca="1" si="2">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:J13" ca="1" si="3">RANDBETWEEN(1,9)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1433,7 +1425,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
@@ -1441,30 +1433,30 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1473,23 +1465,23 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="3"/>
@@ -1497,14 +1489,14 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1513,7 +1505,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -1521,11 +1513,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="3"/>
@@ -1537,14 +1529,14 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1553,7 +1545,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -1561,30 +1553,30 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1593,11 +1585,11 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
@@ -1605,15 +1597,15 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
@@ -1621,10 +1613,10 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1633,7 +1625,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
@@ -1641,19 +1633,19 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
@@ -1661,10 +1653,10 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1673,38 +1665,38 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1713,15 +1705,15 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
@@ -1729,22 +1721,22 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1753,38 +1745,38 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1793,38 +1785,38 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1837,36 +1829,31 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base de datos hecha
</commit_message>
<xml_diff>
--- a/p2/database/dades.xlsx
+++ b/p2/database/dades.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maikell\Documents\Github\ADB\p2\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16608" windowHeight="9432" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="9435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="1" r:id="rId1"/>
@@ -13,10 +18,14 @@
     <sheet name="geografia" sheetId="4" r:id="rId4"/>
     <sheet name="tienda" sheetId="5" r:id="rId5"/>
     <sheet name="ventas" sheetId="6" r:id="rId6"/>
+    <sheet name="sexo" sheetId="7" r:id="rId7"/>
+    <sheet name="categoria" sheetId="8" r:id="rId8"/>
+    <sheet name="articulo" sheetId="9" r:id="rId9"/>
+    <sheet name="campanya" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>Rajah</t>
   </si>
@@ -162,14 +171,85 @@
   </si>
   <si>
     <t>Foot_wear</t>
+  </si>
+  <si>
+    <t>masculino</t>
+  </si>
+  <si>
+    <t>femenino</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>camisetas</t>
+  </si>
+  <si>
+    <t>camisas</t>
+  </si>
+  <si>
+    <t>chaquetas</t>
+  </si>
+  <si>
+    <t>abrigo</t>
+  </si>
+  <si>
+    <t>blusas</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>faldas</t>
+  </si>
+  <si>
+    <t>vaqueros</t>
+  </si>
+  <si>
+    <t>amarillo</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>rojo</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>camp_nike</t>
+  </si>
+  <si>
+    <t>camp_adidas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -197,11 +277,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,26 +554,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -510,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -530,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -550,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -570,7 +653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -590,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -610,7 +693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -630,7 +713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -650,7 +733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -676,20 +759,84 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="3">
+        <v>41570</v>
+      </c>
+      <c r="E1" s="3">
+        <v>41613</v>
+      </c>
+      <c r="F1">
+        <v>123</v>
+      </c>
+      <c r="G1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3">
+        <v>41583</v>
+      </c>
+      <c r="E2" s="3">
+        <v>41599</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -706,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -723,7 +870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -740,7 +887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -757,7 +904,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -774,7 +921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -791,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -808,7 +955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -825,7 +972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -848,165 +995,165 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D1">
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(A1,1)</f>
         <v>2</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B9" ca="1" si="0">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C9" ca="1" si="1">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>2013</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A8" si="2">SUM(A2,1)</f>
         <v>3</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>2013</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>2013</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2013</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>2013</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>SUM(A8,1)</f>
         <v>9</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>2013</v>
@@ -1018,21 +1165,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1049,7 +1196,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(A1,1)</f>
         <v>2</v>
@@ -1067,7 +1214,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">SUM(A2,1)</f>
         <v>3</v>
@@ -1085,7 +1232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1103,7 +1250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1121,7 +1268,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1139,7 +1286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1157,7 +1304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1175,7 +1322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1199,19 +1346,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1222,7 +1369,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -1234,7 +1381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">A2+1</f>
         <v>3</v>
@@ -1246,7 +1393,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1258,7 +1405,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1270,7 +1417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1282,7 +1429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1294,7 +1441,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1306,7 +1453,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1324,19 +1471,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1353,30 +1501,50 @@
       </c>
       <c r="E1">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K1">
+        <f ca="1">RANDBETWEEN(1,9)</f>
+        <v>7</v>
+      </c>
+      <c r="L1">
+        <f ca="1">RANDBETWEEN(1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <f ca="1">RANDBETWEEN(1,8)</f>
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <f ca="1">RANDBETWEEN(1,9)</f>
+        <v>3</v>
+      </c>
+      <c r="O1">
+        <f ca="1">RANDBETWEEN(1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1385,7 +1553,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(10,20)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D13" ca="1" si="1">RANDBETWEEN(1,4)</f>
@@ -1393,30 +1561,50 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E13" ca="1" si="2">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:J13" ca="1" si="3">RANDBETWEEN(1,9)</f>
-        <v>1</v>
+        <f t="shared" ref="F2:K13" ca="1" si="3">RANDBETWEEN(1,9)</f>
+        <v>3</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L13" ca="1" si="4">RANDBETWEEN(1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M13" ca="1" si="5">RANDBETWEEN(1,8)</f>
+        <v>8</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N12" ca="1" si="6">RANDBETWEEN(1,9)</f>
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O13" ca="1" si="7">RANDBETWEEN(1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1425,38 +1613,58 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1465,23 +1673,23 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="3"/>
@@ -1489,14 +1697,34 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1505,38 +1733,58 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="3"/>
         <v>9</v>
       </c>
-      <c r="I5">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
       <c r="J5">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1549,7 +1797,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
@@ -1557,26 +1805,46 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="N6">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1585,38 +1853,58 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1625,38 +1913,58 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1665,7 +1973,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
@@ -1673,30 +1981,50 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1705,7 +2033,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
@@ -1713,30 +2041,50 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1745,7 +2093,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
@@ -1753,15 +2101,15 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="3"/>
         <v>9</v>
       </c>
-      <c r="F11">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
@@ -1769,14 +2117,34 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1785,38 +2153,58 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="O12">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1825,35 +2213,390 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <f ca="1">RANDBETWEEN(1,9)</f>
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="B9:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>9</v>
       </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="3"/>
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>